<commit_message>
Added the 'lower_triangular' matrix as a possible constant.
</commit_message>
<xml_diff>
--- a/default/2_multi_year/concept.xlsx
+++ b/default/2_multi_year/concept.xlsx
@@ -8,73 +8,49 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\2_multi_year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11507919-1833-468B-BBD3-D3ACCE3AD794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81E6717-C5C5-4B10-A7D8-5B241F5A4DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{06EFE0C8-4E47-4609-AC19-51B7AEF26777}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{06EFE0C8-4E47-4609-AC19-51B7AEF26777}"/>
   </bookViews>
   <sheets>
     <sheet name="multi-year" sheetId="4" r:id="rId1"/>
-    <sheet name="variable_no_set" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
-    <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'multi-year'!$I$14:$J$18,'multi-year'!$T$10:$X$11,'multi-year'!$K$33:$L$37</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">variable_no_set!$E$9:$E$13</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'multi-year'!$Z$8:$AD$8</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">variable_no_set!$M$6:$Q$6</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'multi-year'!$Z$10:$AD$11</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'multi-year'!$L$56:$L$60</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'multi-year'!$K$63:$K$67</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'multi-year'!$K$70:$K$74</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'multi-year'!$K$56:$L$60</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'multi-year'!$K$63:$L$67</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'multi-year'!$K$63:$K$67</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'multi-year'!$T$15</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">variable_no_set!$G$16</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -119,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
   <si>
     <t>techs</t>
   </si>
@@ -211,12 +187,6 @@
     <t>capacity, opearative, initial</t>
   </si>
   <si>
-    <t>tech</t>
-  </si>
-  <si>
-    <t>flow</t>
-  </si>
-  <si>
     <t>costs</t>
   </si>
   <si>
@@ -232,9 +202,6 @@
     <t>s.2</t>
   </si>
   <si>
-    <t>availability, equality</t>
-  </si>
-  <si>
     <t>availability, max</t>
   </si>
   <si>
@@ -265,24 +232,12 @@
     <t>X</t>
   </si>
   <si>
-    <t>obj</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
     <t>c_op</t>
   </si>
   <si>
     <t>c_inv</t>
   </si>
   <si>
-    <t>ts_eq</t>
-  </si>
-  <si>
-    <t>ts_bd</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -328,28 +283,19 @@
     <t>h/y</t>
   </si>
   <si>
-    <t>cap_o*diag(ts_eq) - X_eq == 0</t>
-  </si>
-  <si>
     <t>cap_o * diag(ts_min) - X_maxmin &lt;= 0</t>
   </si>
   <si>
     <t>cap_o*diag(ts_max) - X_maxmin &gt;= 0</t>
   </si>
   <si>
-    <t>flow1</t>
-  </si>
-  <si>
-    <t>s.t.</t>
-  </si>
-  <si>
-    <t>u*X' - Y == 0</t>
-  </si>
-  <si>
-    <t>tech1</t>
-  </si>
-  <si>
-    <t>tech2</t>
+    <t>ts_max</t>
+  </si>
+  <si>
+    <t>ts_min</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -359,16 +305,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -402,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -528,44 +468,25 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -575,19 +496,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -597,10 +511,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385CB4FB-63D6-4C57-AD69-C1B6C5EB493E}">
-  <dimension ref="A1:AD74"/>
+  <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W44" sqref="W44:W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1004,7 +924,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <v>1.2</v>
       </c>
     </row>
@@ -1013,10 +933,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
@@ -1046,10 +966,10 @@
         <v>4</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>9</v>
@@ -1069,19 +989,19 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="I7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="Z7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.35">
@@ -1106,67 +1026,67 @@
       <c r="L8" s="1">
         <v>0</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="6">
         <v>100</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="6">
         <f>N8*$N$2</f>
         <v>120</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="6">
         <f t="shared" ref="P8:R8" si="0">O8*$N$2</f>
         <v>144</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="6">
         <f t="shared" si="0"/>
         <v>172.79999999999998</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="6">
         <f t="shared" si="0"/>
         <v>207.35999999999999</v>
       </c>
-      <c r="T8" s="28">
+      <c r="T8" s="6">
         <f t="array" ref="T8:X8">MMULT(I8:J8,TRANSPOSE(I14:J18))</f>
         <v>100.876</v>
       </c>
-      <c r="U8" s="28">
+      <c r="U8" s="6">
         <v>120.876</v>
       </c>
-      <c r="V8" s="28">
+      <c r="V8" s="6">
         <v>144.876</v>
       </c>
-      <c r="W8" s="28">
+      <c r="W8" s="6">
         <v>176.876</v>
       </c>
-      <c r="X8" s="28">
+      <c r="X8" s="6">
         <v>215.27600000000001</v>
       </c>
-      <c r="Z8" s="16">
+      <c r="Z8" s="11">
         <f t="array" ref="Z8:AD8">T8:X8-MMULT(K8:L8,T10:X11)-N8:R8</f>
         <v>0</v>
       </c>
-      <c r="AA8" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="17">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="17">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="18">
+      <c r="AA8" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="12">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="I9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="T9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Z9" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.35">
@@ -1182,35 +1102,35 @@
       <c r="J10" s="1">
         <v>0</v>
       </c>
-      <c r="T10" s="14">
+      <c r="T10" s="9">
         <v>8.76</v>
       </c>
-      <c r="U10" s="14">
+      <c r="U10" s="9">
         <v>8.76</v>
       </c>
-      <c r="V10" s="14">
+      <c r="V10" s="9">
         <v>8.76</v>
       </c>
-      <c r="W10" s="14">
+      <c r="W10" s="9">
         <v>40.76</v>
       </c>
-      <c r="X10" s="14">
+      <c r="X10" s="9">
         <v>79.16</v>
       </c>
-      <c r="Z10" s="19">
+      <c r="Z10" s="14">
         <f t="array" ref="Z10:AD11">T10:X11-MMULT(I10:J11,TRANSPOSE(I14:J18))</f>
         <v>0</v>
       </c>
-      <c r="AA10" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="20">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="20">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="21">
+      <c r="AA10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="16">
         <v>0</v>
       </c>
     </row>
@@ -1227,82 +1147,82 @@
       <c r="J11" s="1">
         <v>1</v>
       </c>
-      <c r="T11" s="14">
+      <c r="T11" s="9">
         <v>92.116</v>
       </c>
-      <c r="U11" s="14">
+      <c r="U11" s="9">
         <v>112.116</v>
       </c>
-      <c r="V11" s="14">
+      <c r="V11" s="9">
         <v>136.11600000000001</v>
       </c>
-      <c r="W11" s="14">
+      <c r="W11" s="9">
         <v>136.11600000000001</v>
       </c>
-      <c r="X11" s="14">
+      <c r="X11" s="9">
         <v>136.11600000000001</v>
       </c>
-      <c r="Z11" s="22">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="23">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="24">
+      <c r="Z11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="I13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="9">
         <v>8.76</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="9">
         <v>92.116</v>
       </c>
       <c r="T14" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="9">
         <v>8.76</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="9">
         <v>112.116</v>
       </c>
-      <c r="T15" s="12" cm="1">
+      <c r="T15" s="7" cm="1">
         <f t="array" ref="T15">SUM(K42:L46+K49:L53)</f>
-        <v>97970.740642999983</v>
+        <v>97970.740642999997</v>
       </c>
       <c r="U15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="9">
         <v>8.76</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="9">
         <v>136.11600000000001</v>
       </c>
     </row>
@@ -1310,10 +1230,10 @@
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="9">
         <v>40.76</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="9">
         <v>136.11600000000001</v>
       </c>
     </row>
@@ -1321,115 +1241,112 @@
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="9">
         <v>79.16</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="9">
         <v>136.11600000000001</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="1">
-        <v>150</v>
-      </c>
-      <c r="L20" s="1">
-        <v>0</v>
-      </c>
-      <c r="M20" t="s">
-        <v>50</v>
+      <c r="K20" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="1">
+        <v>150</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
         <v>17</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>25</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K22" s="1">
         <v>700</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L22" s="1">
         <v>700</v>
       </c>
-      <c r="M21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="K22" t="s">
-        <v>43</v>
+      <c r="M22" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" t="s">
-        <v>68</v>
-      </c>
-      <c r="L23" s="1">
-        <f>0.15*8760</f>
-        <v>1314</v>
-      </c>
-      <c r="M23" t="s">
-        <v>52</v>
+      <c r="K23" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="E24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H24" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="K24" s="1">
         <f>0.9*8760</f>
         <v>7884</v>
       </c>
+      <c r="L24" s="1">
+        <f>0.15*8760</f>
+        <v>1314</v>
+      </c>
       <c r="M24" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="E25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H25" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="K25" s="1">
         <f>0.2*8760</f>
         <v>1752</v>
       </c>
+      <c r="L25" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M25" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="K26" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="T26" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.35">
@@ -1443,7 +1360,7 @@
         <v>27</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K27" s="4">
         <f t="array" ref="K27:L31">K39:L39+MMULT(T27:X31,K33:L37)</f>
@@ -1476,7 +1393,7 @@
         <v>5</v>
       </c>
       <c r="L28" s="4">
-        <v>85.324200999999988</v>
+        <v>103.58904099999999</v>
       </c>
       <c r="T28" s="1">
         <v>1</v>
@@ -1502,7 +1419,7 @@
         <v>5</v>
       </c>
       <c r="L29" s="4">
-        <v>103.58904099999998</v>
+        <v>103.58904099999999</v>
       </c>
       <c r="T29" s="1">
         <v>1</v>
@@ -1528,7 +1445,7 @@
         <v>5.1699644899999999</v>
       </c>
       <c r="L30" s="4">
-        <v>103.58904099999998</v>
+        <v>103.58904099999999</v>
       </c>
       <c r="T30" s="1">
         <v>1</v>
@@ -1554,7 +1471,7 @@
         <v>10.040588490000001</v>
       </c>
       <c r="L31" s="4">
-        <v>103.58904099999998</v>
+        <v>103.58904099999999</v>
       </c>
       <c r="T31" s="1">
         <v>1</v>
@@ -1574,9 +1491,9 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="K32" t="s">
-        <v>44</v>
-      </c>
-      <c r="L32" s="13"/>
+        <v>41</v>
+      </c>
+      <c r="L32" s="8"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
@@ -1589,12 +1506,12 @@
         <v>28</v>
       </c>
       <c r="H33" t="s">
-        <v>46</v>
-      </c>
-      <c r="K33" s="15">
-        <v>0</v>
-      </c>
-      <c r="L33" s="15">
+        <v>43</v>
+      </c>
+      <c r="K33" s="10">
+        <v>0</v>
+      </c>
+      <c r="L33" s="10">
         <v>70.103500999999994</v>
       </c>
     </row>
@@ -1602,32 +1519,32 @@
       <c r="A34" t="s">
         <v>20</v>
       </c>
-      <c r="K34" s="15">
-        <v>0</v>
-      </c>
-      <c r="L34" s="15">
-        <v>15.220700000000001</v>
+      <c r="K34" s="10">
+        <v>0</v>
+      </c>
+      <c r="L34" s="10">
+        <v>33.48554</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>21</v>
       </c>
-      <c r="K35" s="15">
-        <v>0</v>
-      </c>
-      <c r="L35" s="15">
-        <v>18.26484</v>
+      <c r="K35" s="10">
+        <v>0</v>
+      </c>
+      <c r="L35" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>22</v>
       </c>
-      <c r="K36" s="15">
+      <c r="K36" s="10">
         <v>0.16996449</v>
       </c>
-      <c r="L36" s="15">
+      <c r="L36" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1635,16 +1552,16 @@
       <c r="A37" t="s">
         <v>23</v>
       </c>
-      <c r="K37" s="15">
+      <c r="K37" s="10">
         <v>4.8706240000000003</v>
       </c>
-      <c r="L37" s="15">
+      <c r="L37" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
@@ -1655,7 +1572,7 @@
         <v>29</v>
       </c>
       <c r="H39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K39" s="1">
         <v>5</v>
@@ -1666,7 +1583,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K41" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
@@ -1674,7 +1591,7 @@
         <v>19</v>
       </c>
       <c r="K42" s="1">
-        <f t="array" ref="K42:L46">MMULT(TRANSPOSE(T10:X11),_xlfn.MUNIT(2)*K20:L20)</f>
+        <f t="array" ref="K42:L46">MMULT(TRANSPOSE(T10:X11),_xlfn.MUNIT(2)*K21:L21)</f>
         <v>1314</v>
       </c>
       <c r="L42" s="1">
@@ -1727,7 +1644,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K48" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
@@ -1735,7 +1652,7 @@
         <v>19</v>
       </c>
       <c r="K49" s="1">
-        <f t="array" ref="K49:L53">K21:L21*K33:L37</f>
+        <f t="array" ref="K49:L53">K22:L22*K33:L37</f>
         <v>0</v>
       </c>
       <c r="L49" s="1">
@@ -1750,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="L50" s="1">
-        <v>10654.49</v>
+        <v>23439.878000000001</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
@@ -1761,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="L51" s="1">
-        <v>12785.387999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
@@ -1788,15 +1705,18 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K55" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>19</v>
       </c>
+      <c r="K56" s="24">
+        <f t="array" ref="K56:L60">MMULT(K27:L31,_xlfn.MUNIT(2)*K24:L24)*0.001- TRANSPOSE(T10:X11)</f>
+        <v>30.660000000000004</v>
+      </c>
       <c r="L56" s="25">
-        <f t="array" ref="L56:L60">MMULT(L27:L31,_xlfn.MUNIT(1)*L23)*0.001 - TRANSPOSE(T11:X11)</f>
         <v>3.1399999045333971E-7</v>
       </c>
     </row>
@@ -1804,325 +1724,110 @@
       <c r="A57" t="s">
         <v>20</v>
       </c>
-      <c r="L57" s="26">
-        <v>1.1399998811612022E-7</v>
+      <c r="K57" s="26">
+        <v>30.660000000000004</v>
+      </c>
+      <c r="L57" s="27">
+        <v>23.999999874000011</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>21</v>
       </c>
-      <c r="L58" s="26">
-        <v>-1.2600003174156882E-7</v>
+      <c r="K58" s="26">
+        <v>30.660000000000004</v>
+      </c>
+      <c r="L58" s="27">
+        <v>-1.2600000331985939E-7</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>22</v>
       </c>
-      <c r="L59" s="26">
-        <v>-1.2600003174156882E-7</v>
+      <c r="K59" s="26">
+        <v>3.915999968739925E-8</v>
+      </c>
+      <c r="L59" s="27">
+        <v>-1.2600000331985939E-7</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>23</v>
       </c>
-      <c r="L60" s="27">
-        <v>-1.2600003174156882E-7</v>
+      <c r="K60" s="28">
+        <v>-3.4483998945233907E-7</v>
+      </c>
+      <c r="L60" s="29">
+        <v>-1.2600000331985939E-7</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K62" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>19</v>
       </c>
-      <c r="K63" s="25">
-        <f t="array" ref="K63:K67">MMULT(K27:K31,_xlfn.MUNIT(1)*K24)*0.001- TRANSPOSE(T10:X10)</f>
-        <v>30.660000000000004</v>
+      <c r="K63" s="14">
+        <f t="array" ref="K63:L67">MMULT(K27:L31,_xlfn.MUNIT(2)*K25:L25)*0.001- TRANSPOSE(T10:X11)</f>
+        <v>0</v>
+      </c>
+      <c r="L63" s="20">
+        <v>-22.012499000000005</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>20</v>
       </c>
-      <c r="K64" s="26">
-        <v>30.660000000000004</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K64" s="21">
+        <v>0</v>
+      </c>
+      <c r="L64" s="22">
+        <v>-8.5269590000000051</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>21</v>
       </c>
-      <c r="K65" s="26">
-        <v>30.660000000000004</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K65" s="21">
+        <v>0</v>
+      </c>
+      <c r="L65" s="22">
+        <v>-32.526959000000019</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>22</v>
       </c>
-      <c r="K66" s="26">
-        <v>3.915999968739925E-8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K66" s="21">
+        <v>-31.702222213519999</v>
+      </c>
+      <c r="L66" s="22">
+        <v>-32.526959000000019</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>23</v>
       </c>
-      <c r="K67" s="27">
-        <v>-3.4483998945233907E-7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="K69" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>19</v>
-      </c>
-      <c r="K70" s="25">
-        <f t="array" ref="K70:K74">MMULT(K27:K31,_xlfn.MUNIT(1)*K25)*0.001- TRANSPOSE(T10:X10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>20</v>
-      </c>
-      <c r="K71" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>21</v>
-      </c>
-      <c r="K72" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>22</v>
-      </c>
-      <c r="K73" s="26">
-        <v>-31.702222213519999</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>23</v>
-      </c>
-      <c r="K74" s="27">
+      <c r="K67" s="17">
         <v>-61.568888965519989</v>
+      </c>
+      <c r="L67" s="23">
+        <v>-32.526959000000019</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0414D2E3-55F0-473F-97D1-99585BE4E019}">
-  <dimension ref="A1:Q17"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="3" width="6.453125" customWidth="1"/>
-    <col min="5" max="21" width="5.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>2</v>
-      </c>
-      <c r="I6" s="1">
-        <v>3</v>
-      </c>
-      <c r="J6" s="1">
-        <v>4</v>
-      </c>
-      <c r="K6" s="1">
-        <v>5</v>
-      </c>
-      <c r="M6" s="9">
-        <f t="array" ref="M6:Q6">MMULT(E6,TRANSPOSE(E9:E13))-G6:K6</f>
-        <v>-1.0000000050247593E-8</v>
-      </c>
-      <c r="N6" s="10">
-        <v>9.9999999392252903E-9</v>
-      </c>
-      <c r="O6" s="10">
-        <v>0</v>
-      </c>
-      <c r="P6" s="10">
-        <v>-1.0000000028043132E-7</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>1.0000000028043132E-7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="8">
-        <v>3.3333333000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="8">
-        <v>6.6666667000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="8">
-        <v>13.333333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="8">
-        <v>16.666667</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding 'default\2_multi_year' problem (not working). Code refactoring required. Last commit before branching.
</commit_message>
<xml_diff>
--- a/default/2_multi_year/concept.xlsx
+++ b/default/2_multi_year/concept.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\2_multi_year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81E6717-C5C5-4B10-A7D8-5B241F5A4DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52209A2-3465-47B5-A99F-049A4342725E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{06EFE0C8-4E47-4609-AC19-51B7AEF26777}"/>
+    <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
   </bookViews>
   <sheets>
     <sheet name="multi-year" sheetId="4" r:id="rId1"/>
+    <sheet name="problem" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="96">
   <si>
     <t>techs</t>
   </si>
@@ -250,12 +251,6 @@
     <t>d</t>
   </si>
   <si>
-    <t>X - d*Q == 0</t>
-  </si>
-  <si>
-    <t>Q_agg == I*Q</t>
-  </si>
-  <si>
     <t>Q_agg - u*X - Y == 0</t>
   </si>
   <si>
@@ -283,12 +278,6 @@
     <t>h/y</t>
   </si>
   <si>
-    <t>cap_o * diag(ts_min) - X_maxmin &lt;= 0</t>
-  </si>
-  <si>
-    <t>cap_o*diag(ts_max) - X_maxmin &gt;= 0</t>
-  </si>
-  <si>
     <t>ts_max</t>
   </si>
   <si>
@@ -296,6 +285,105 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>all sets</t>
+  </si>
+  <si>
+    <t>set-inter</t>
+  </si>
+  <si>
+    <t>set-intra</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>sum_vector</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>scenarios</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>tecnologies</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>technical specs</t>
+  </si>
+  <si>
+    <t>lower_triangular</t>
+  </si>
+  <si>
+    <t>y,y</t>
+  </si>
+  <si>
+    <t>1,f</t>
+  </si>
+  <si>
+    <t>exogenous</t>
+  </si>
+  <si>
+    <t>f,t</t>
+  </si>
+  <si>
+    <t>market shares coef.</t>
+  </si>
+  <si>
+    <t>use coef.</t>
+  </si>
+  <si>
+    <t>s,t,f</t>
+  </si>
+  <si>
+    <t>t,f</t>
+  </si>
+  <si>
+    <t>Q_agg == I*Q'</t>
+  </si>
+  <si>
+    <t>X - d*Q' == 0</t>
+  </si>
+  <si>
+    <t>cap_o*diag(ts_max) - X &gt;= 0</t>
+  </si>
+  <si>
+    <t>cap_o * diag(ts_min) - X &lt;= 0</t>
   </si>
 </sst>
 </file>
@@ -857,17 +945,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385CB4FB-63D6-4C57-AD69-C1B6C5EB493E}">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W44" sqref="W44:W45"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="6" width="6.54296875" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.54296875" customWidth="1"/>
-    <col min="9" max="30" width="5.81640625" customWidth="1"/>
-    <col min="31" max="34" width="5.08984375" customWidth="1"/>
+    <col min="9" max="48" width="6.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.35">
@@ -989,7 +1074,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="I7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s">
         <v>38</v>
@@ -998,10 +1083,10 @@
         <v>39</v>
       </c>
       <c r="T7" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="Z7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.35">
@@ -1086,7 +1171,7 @@
         <v>44</v>
       </c>
       <c r="Z9" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.35">
@@ -1194,7 +1279,7 @@
         <v>92.116</v>
       </c>
       <c r="T14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.35">
@@ -1212,7 +1297,7 @@
         <v>97970.740642999997</v>
       </c>
       <c r="U15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.35">
@@ -1250,7 +1335,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="K20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
@@ -1306,7 +1391,7 @@
         <v>35</v>
       </c>
       <c r="H24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K24" s="1">
         <f>0.9*8760</f>
@@ -1317,7 +1402,7 @@
         <v>1314</v>
       </c>
       <c r="M24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.35">
@@ -1328,7 +1413,7 @@
         <v>37</v>
       </c>
       <c r="H25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K25" s="1">
         <f>0.2*8760</f>
@@ -1338,15 +1423,15 @@
         <v>1000</v>
       </c>
       <c r="M25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="K26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.35">
@@ -1565,9 +1650,6 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
       <c r="G39" t="s">
         <v>29</v>
       </c>
@@ -1583,7 +1665,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
@@ -1644,7 +1726,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K48" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
@@ -1705,7 +1787,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K55" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
@@ -1766,7 +1848,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K62" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
@@ -1831,16 +1913,182 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7B19A0-9389-4FEF-964D-37897EE28C1D}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D81D9CE2A426814A9054AC6C4C722ED5" ma:contentTypeVersion="10" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="df56dec458b733a6f5a4aa88128e48ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aa97a2c6-5066-49ad-90c0-e23f9da31bb2" xmlns:ns3="c319d79e-6821-4c2a-8db8-88a02643e5e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="57b3dd0920a9f069281dfcd1579251e0" ns2:_="" ns3:_="">
     <xsd:import namespace="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
@@ -2029,15 +2277,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{089C9D8A-2D45-412A-B3BB-E98542CFDEB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C420B358-E840-48FD-BF6F-9DC922742EA6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2054,4 +2303,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{089C9D8A-2D45-412A-B3BB-E98542CFDEB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Variables refactoring: work in progress. Still issue in problem definition.
</commit_message>
<xml_diff>
--- a/default/2_multi_year/concept.xlsx
+++ b/default/2_multi_year/concept.xlsx
@@ -2,55 +2,90 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\2_multi_year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52209A2-3465-47B5-A99F-049A4342725E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A909CE-E904-42EE-84B1-B5336A1F1EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
+    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{0A3BC822-FD99-4F89-AC4E-FBD077FFAF78}"/>
   </bookViews>
   <sheets>
-    <sheet name="multi-year" sheetId="4" r:id="rId1"/>
-    <sheet name="problem" sheetId="5" r:id="rId2"/>
+    <sheet name="multi-year_rcot" sheetId="4" r:id="rId1"/>
+    <sheet name="multi-year" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'multi-year'!$I$14:$J$18,'multi-year'!$T$10:$X$11,'multi-year'!$K$33:$L$37</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'multi-year'!$G$17:$H$21,'multi-year'!$S$11:$W$12</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'multi-year_rcot'!$I$14:$J$18,'multi-year_rcot'!$T$10:$X$11,'multi-year_rcot'!$K$33:$L$37</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'multi-year'!$Z$8:$AD$8</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'multi-year'!$Z$10:$AD$11</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'multi-year'!$K$56:$L$60</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'multi-year'!$K$63:$L$67</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'multi-year'!$K$63:$K$67</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'multi-year'!$Y$8:$AC$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'multi-year_rcot'!$Z$8:$AD$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'multi-year'!$Y$11:$AC$12</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'multi-year_rcot'!$Z$10:$AD$11</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'multi-year'!#REF!</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'multi-year_rcot'!$K$56:$L$60</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'multi-year'!#REF!</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'multi-year_rcot'!$K$63:$L$67</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'multi-year'!#REF!</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'multi-year_rcot'!$K$63:$K$67</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'multi-year'!$T$15</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'multi-year'!$S$18</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'multi-year_rcot'!$T$15</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -96,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="69">
   <si>
     <t>techs</t>
   </si>
@@ -287,93 +322,9 @@
     <t>c</t>
   </si>
   <si>
-    <t>shape</t>
-  </si>
-  <si>
-    <t>symbol</t>
-  </si>
-  <si>
-    <t>all sets</t>
-  </si>
-  <si>
-    <t>set-inter</t>
-  </si>
-  <si>
-    <t>set-intra</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>constant</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>sum_vector</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>scenarios</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>sensitivity</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>tecnologies</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>technical specs</t>
-  </si>
-  <si>
-    <t>lower_triangular</t>
-  </si>
-  <si>
-    <t>y,y</t>
-  </si>
-  <si>
-    <t>1,f</t>
-  </si>
-  <si>
-    <t>exogenous</t>
-  </si>
-  <si>
-    <t>f,t</t>
-  </si>
-  <si>
-    <t>market shares coef.</t>
-  </si>
-  <si>
-    <t>use coef.</t>
-  </si>
-  <si>
-    <t>s,t,f</t>
-  </si>
-  <si>
-    <t>t,f</t>
-  </si>
-  <si>
     <t>Q_agg == I*Q'</t>
   </si>
   <si>
@@ -384,6 +335,9 @@
   </si>
   <si>
     <t>cap_o * diag(ts_min) - X &lt;= 0</t>
+  </si>
+  <si>
+    <t>Q' - u*X - Y == 0</t>
   </si>
 </sst>
 </file>
@@ -393,7 +347,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,8 +369,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +386,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -609,6 +581,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,9 +918,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385CB4FB-63D6-4C57-AD69-C1B6C5EB493E}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R47" sqref="R47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1083,7 +1061,7 @@
         <v>39</v>
       </c>
       <c r="T7" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="Z7" t="s">
         <v>51</v>
@@ -1171,7 +1149,7 @@
         <v>44</v>
       </c>
       <c r="Z9" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.35">
@@ -1787,7 +1765,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K55" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
@@ -1848,7 +1826,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K62" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
@@ -1914,177 +1892,520 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7B19A0-9389-4FEF-964D-37897EE28C1D}">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B9C269-8EBE-47B7-80AA-01E8CD0CCD53}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:AC28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="1" max="4" width="6.54296875" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" customWidth="1"/>
+    <col min="7" max="47" width="6.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="5">
+        <v>1.2</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="31">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
+      <c r="H8" s="31">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <f>M8*$N$7</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="6">
+        <f>N8*$N$7</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="6">
+        <f>O8*$N$7</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="6">
+        <f>P8*$N$7</f>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="14">
+        <f t="array" ref="Y8:AC9">TRANSPOSE(G17:H21)-MMULT(J8:K9,S11:W12)-M8:Q9</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="31">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <v>100</v>
+      </c>
+      <c r="N9" s="6">
+        <f>M9*$N$7</f>
+        <v>120</v>
+      </c>
+      <c r="O9" s="6">
+        <f>N9*$N$7</f>
+        <v>144</v>
+      </c>
+      <c r="P9" s="6">
+        <f>O9*$N$7</f>
+        <v>172.79999999999998</v>
+      </c>
+      <c r="Q9" s="6">
+        <f>P9*$N$7</f>
+        <v>207.35999999999999</v>
+      </c>
+      <c r="Y9" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="S10" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="30">
+        <v>0</v>
+      </c>
+      <c r="T11" s="30">
+        <v>0</v>
+      </c>
+      <c r="U11" s="30">
+        <v>0</v>
+      </c>
+      <c r="V11" s="30">
+        <v>0</v>
+      </c>
+      <c r="W11" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="14">
+        <f t="array" ref="Y11:AC12">S11:W12-MMULT(G11:H12,TRANSPOSE(G17:H21))</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="S12" s="30">
+        <v>100</v>
+      </c>
+      <c r="T12" s="30">
+        <v>120</v>
+      </c>
+      <c r="U12" s="30">
+        <v>144</v>
+      </c>
+      <c r="V12" s="30">
+        <v>172.8</v>
+      </c>
+      <c r="W12" s="30">
+        <v>207.36</v>
+      </c>
+      <c r="Y12" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="J13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="1">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" t="s">
-        <v>91</v>
+      <c r="K14" s="1">
+        <v>20</v>
+      </c>
+      <c r="L14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="30">
+        <v>0</v>
+      </c>
+      <c r="H17" s="30">
+        <v>100</v>
+      </c>
+      <c r="S17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="30">
+        <v>0</v>
+      </c>
+      <c r="H18" s="30">
+        <v>120</v>
+      </c>
+      <c r="S18" s="7">
+        <v>1</v>
+      </c>
+      <c r="T18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="30">
+        <v>0</v>
+      </c>
+      <c r="H19" s="30">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="30">
+        <v>0</v>
+      </c>
+      <c r="H20" s="30">
+        <v>172.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="30">
+        <v>0</v>
+      </c>
+      <c r="H21" s="30">
+        <v>207.36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J24" s="32">
+        <f t="array" ref="J24:K28">MMULT(TRANSPOSE(S11:W12),_xlfn.MUNIT(2)*J14:K14)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="32">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="32">
+        <v>0</v>
+      </c>
+      <c r="K25" s="32">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="32">
+        <v>0</v>
+      </c>
+      <c r="K26" s="32">
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="32">
+        <v>0</v>
+      </c>
+      <c r="K27" s="32">
+        <v>3456</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="32">
+        <v>0</v>
+      </c>
+      <c r="K28" s="32">
+        <v>4147.2000000000007</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>